<commit_message>
Update .gitignore and modify/delete some files
</commit_message>
<xml_diff>
--- a/static/pelanggaran_log.xlsx
+++ b/static/pelanggaran_log.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -463,22 +463,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>30 June 2025</t>
+          <t>05 July 2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>19:08:49</t>
+          <t>12:17:02</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>M9</t>
+          <t>M16</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -488,71 +488,71 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>85.78</t>
+          <t>60.07</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>pelanggaran_20250630_190849.jpg</t>
+          <t>pelanggaran_20250705_121702.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>30 June 2025</t>
+          <t>05 July 2025</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>19:08:49</t>
+          <t>12:17:02</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>B6</t>
+          <t>M17</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>motor</t>
+          <t>mobil</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>85.78</t>
+          <t>60.07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>pelanggaran_20250630_190849.jpg</t>
+          <t>pelanggaran_20250705_121702.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01 July 2025</t>
+          <t>05 July 2025</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>19:16:46</t>
+          <t>12:17:02</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>M19</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -562,12 +562,123 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>69.36</t>
+          <t>60.07</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>pelanggaran_20250701_191646.jpg</t>
+          <t>pelanggaran_20250705_121702.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>05 July 2025</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12:17:02</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>M23</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>mobil</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>60.07</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>pelanggaran_20250705_121702.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05 July 2025</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12:24:54</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>M24</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>mobil</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>79.27</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>pelanggaran_20250705_122454.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05 July 2025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>13:43:56</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>M112</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>mobil</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>42.60</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>pelanggaran_20250705_134356.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>